<commit_message>
Mejoras, eliminacion de imagenes en edicion
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -643,19 +643,27 @@
           <t>sello caballero oro 18 k y piedra roja rubi</t>
         </is>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>1800</v>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>(vacio)</t>
-        </is>
-      </c>
-      <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>1800</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="7" t="inlineStr">
@@ -668,18 +676,26 @@
           <t>sello caballero oro 18 k y piedra roja rubi</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E6" s="7" t="inlineStr">
-        <is>
-          <t>(vacio)</t>
-        </is>
-      </c>
-      <c r="F6" s="7" t="n"/>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F6" s="9" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
       <c r="G6" s="7" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
@@ -2667,6 +2683,10 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G3" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" r:id="rId6"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregados estilos a los templates e incorporacion de mas imagenes de objetos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1070,11 +1070,25 @@
           <t>correa reloj oro 18 k</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>38</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1000</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1088,11 +1102,30 @@
           <t>reloj cyma de oro antiguo</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>33</v>
-      </c>
-      <c r="D21" t="n">
-        <v>600</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1106,11 +1139,30 @@
           <t>pulsera rigida oro 18 k labrada</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>58</v>
-      </c>
-      <c r="D22" t="n">
-        <v>6000</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -2270,6 +2322,14 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId37"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E19" r:id="rId38"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E20" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E21" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G21" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E22" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G22" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refinando popup e incorporando fotos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1176,11 +1176,30 @@
           <t>pulsera rigida oro 18 k labrada</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>54</v>
-      </c>
-      <c r="D23" t="n">
-        <v>6000</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -2330,6 +2349,9 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E22" r:id="rId45"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId46"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G22" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E23" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G23" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
eliminacion de imagenes incorporadas
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1860,8 +1860,20 @@
           <t>reloj omega sra. Constelacion</t>
         </is>
       </c>
-      <c r="D45" t="n">
-        <v>8000</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1875,11 +1887,30 @@
           <t>sortija  oro amarillo y blanco con un gran diamante</t>
         </is>
       </c>
-      <c r="C46" t="n">
-        <v>2</v>
-      </c>
-      <c r="D46" t="n">
-        <v>2000</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G46" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1893,11 +1924,20 @@
           <t>placa eugenio de frutos oro</t>
         </is>
       </c>
-      <c r="C47" t="n">
-        <v>3</v>
-      </c>
-      <c r="D47" t="n">
-        <v>240</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1911,11 +1951,25 @@
           <t>anillo de oro blanco y diamantes</t>
         </is>
       </c>
-      <c r="C48" t="n">
-        <v>5</v>
-      </c>
-      <c r="D48" t="n">
-        <v>1500</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1929,11 +1983,20 @@
           <t>pendientes oro blanco y diamante</t>
         </is>
       </c>
-      <c r="C49" t="n">
-        <v>5</v>
-      </c>
-      <c r="D49" t="n">
-        <v>1500</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1947,11 +2010,20 @@
           <t>pendientes oro blanco y brillantes largos</t>
         </is>
       </c>
-      <c r="C50" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" t="n">
-        <v>800</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1965,11 +2037,20 @@
           <t xml:space="preserve">pulsera oro blanco y circonitas </t>
         </is>
       </c>
-      <c r="C51" t="n">
-        <v>14</v>
-      </c>
-      <c r="D51" t="n">
-        <v>1500</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1983,11 +2064,20 @@
           <t xml:space="preserve">3 pulseras oro </t>
         </is>
       </c>
-      <c r="C52" t="n">
-        <v>38</v>
-      </c>
-      <c r="D52" t="n">
-        <v>3000</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -2001,11 +2091,25 @@
           <t>pulsera antigua oro amarillo y blanco con brillantes</t>
         </is>
       </c>
-      <c r="C53" t="n">
-        <v>6</v>
-      </c>
-      <c r="D53" t="n">
-        <v>2500</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -2019,11 +2123,25 @@
           <t xml:space="preserve">cadena y colgante oro blanco con diamantesy perla </t>
         </is>
       </c>
-      <c r="C54" t="n">
-        <v>8</v>
-      </c>
-      <c r="D54" t="n">
-        <v>2500</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -2037,11 +2155,20 @@
           <t>cadena y cruz oro (papa)</t>
         </is>
       </c>
-      <c r="C55" t="n">
-        <v>16</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1300</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -2055,11 +2182,20 @@
           <t xml:space="preserve">cadena oro y colgante tous </t>
         </is>
       </c>
-      <c r="C56" t="n">
-        <v>8</v>
-      </c>
-      <c r="D56" t="n">
-        <v>300</v>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -2073,11 +2209,20 @@
           <t>cadena y cruz oeo blanco (boda)</t>
         </is>
       </c>
-      <c r="C57" t="n">
-        <v>6</v>
-      </c>
-      <c r="D57" t="n">
-        <v>300</v>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -2091,11 +2236,20 @@
           <t>medalla virgen y cruz con cadena oro 18 k (Mari)</t>
         </is>
       </c>
-      <c r="C58" t="n">
-        <v>15</v>
-      </c>
-      <c r="D58" t="n">
-        <v>1200</v>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -2109,11 +2263,20 @@
           <t>pulsera oro 18 k y perlas (Mari)</t>
         </is>
       </c>
-      <c r="C59" t="n">
-        <v>10</v>
-      </c>
-      <c r="D59" t="n">
-        <v>600</v>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -2127,11 +2290,20 @@
           <t>pulsera aro oro 18 k (regalo Tere)</t>
         </is>
       </c>
-      <c r="C60" t="n">
-        <v>9</v>
-      </c>
-      <c r="D60" t="n">
-        <v>500</v>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -2145,11 +2317,20 @@
           <t xml:space="preserve">Gargantilla trenzada oro 18 k </t>
         </is>
       </c>
-      <c r="C61" t="n">
-        <v>8</v>
-      </c>
-      <c r="D61" t="n">
-        <v>600</v>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="E61" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -2163,11 +2344,20 @@
           <t>gargantilla perlas de rio con broche de oro</t>
         </is>
       </c>
-      <c r="C62" t="n">
-        <v>15</v>
-      </c>
-      <c r="D62" t="n">
-        <v>200</v>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -2181,11 +2371,20 @@
           <t>cadena y cruz pequeña oro 18 k</t>
         </is>
       </c>
-      <c r="C63" t="n">
-        <v>2</v>
-      </c>
-      <c r="D63" t="n">
-        <v>160</v>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -2199,11 +2398,25 @@
           <t>anillo de oro blanco y amarillo 3 brillantes</t>
         </is>
       </c>
-      <c r="C64" t="n">
-        <v>3</v>
-      </c>
-      <c r="D64" t="n">
-        <v>1200</v>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -2217,11 +2430,20 @@
           <t>sortija oro 18k circonitas y rubis</t>
         </is>
       </c>
-      <c r="C65" t="n">
-        <v>3</v>
-      </c>
-      <c r="D65" t="n">
-        <v>240</v>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -2235,11 +2457,25 @@
           <t>sortija oro 18k aro grueso</t>
         </is>
       </c>
-      <c r="C66" t="n">
-        <v>11</v>
-      </c>
-      <c r="D66" t="n">
-        <v>880</v>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>880</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -2253,11 +2489,25 @@
           <t>sortija oro 18k  y circonitas (joyeria Juanjo)</t>
         </is>
       </c>
-      <c r="C67" t="n">
-        <v>5</v>
-      </c>
-      <c r="D67" t="n">
-        <v>400</v>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="E67" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F67" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -2271,11 +2521,25 @@
           <t>solitario oro 18k  con un brillante (joyeria Juanjo)</t>
         </is>
       </c>
-      <c r="C68" t="n">
-        <v>3</v>
-      </c>
-      <c r="D68" t="n">
-        <v>600</v>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="E68" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F68" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -2289,11 +2553,25 @@
           <t>sello oro 18k EG (papa)</t>
         </is>
       </c>
-      <c r="C69" t="n">
-        <v>20</v>
-      </c>
-      <c r="D69" t="n">
-        <v>1600</v>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1600</t>
+        </is>
+      </c>
+      <c r="E69" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F69" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -2307,11 +2585,25 @@
           <t>sortija oro blabco y amarillo con circonitas</t>
         </is>
       </c>
-      <c r="C70" t="n">
-        <v>6</v>
-      </c>
-      <c r="D70" t="n">
-        <v>400</v>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="E70" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F70" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -2804,21 +3096,58 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F43" r:id="rId85"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E44" r:id="rId86"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F44" r:id="rId87"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E71" r:id="rId88"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E73" r:id="rId89"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F73" r:id="rId90"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E74" r:id="rId91"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E75" r:id="rId92"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E76" r:id="rId93"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E77" r:id="rId94"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E78" r:id="rId95"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E79" r:id="rId96"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E80" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E81" r:id="rId98"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E82" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E83" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E84" r:id="rId101"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E85" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E45" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E46" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F46" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G46" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E47" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E48" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F48" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E49" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E50" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E51" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E52" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E53" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F53" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E54" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F54" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E55" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E56" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E57" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E58" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E59" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E60" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E61" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E62" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E63" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E64" r:id="rId112"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F64" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E65" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E66" r:id="rId115"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F66" r:id="rId116"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E67" r:id="rId117"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F67" r:id="rId118"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E68" r:id="rId119"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F68" r:id="rId120"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E69" r:id="rId121"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F69" r:id="rId122"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E70" r:id="rId123"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F70" r:id="rId124"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E71" r:id="rId125"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E73" r:id="rId126"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F73" r:id="rId127"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E74" r:id="rId128"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E75" r:id="rId129"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E76" r:id="rId130"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E77" r:id="rId131"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E78" r:id="rId132"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E79" r:id="rId133"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E80" r:id="rId134"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E81" r:id="rId135"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E82" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E83" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E84" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E85" r:id="rId139"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>